<commit_message>
feat: some new templates for like and in
</commit_message>
<xml_diff>
--- a/dataset/templates.xlsx
+++ b/dataset/templates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2116" uniqueCount="972">
   <si>
     <t>一家医院调取患者之前在其他所有医院的就诊、检查数据，医保对可疑的就诊调取医院的就诊信息，与医保数据进行比对</t>
   </si>
@@ -2425,6 +2425,686 @@
   </si>
   <si>
     <t>SELECT (SELECT SUM(STA_FLG) FROM t_kc22 WHERE MED_CLINIC_ID = $1) = (SELECT COUNT(*) FROM t_kc22 WHERE MED_CLINIC_ID = $1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中就诊科室名称包含某关键字的所有医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员ID）在医院（医疗机构代码）中就诊科室名称包含（部分科室名称）的所有医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM t_kc21 WHERE PERSON_ID = $1 AND MED_SER_ORG_NO = $2 AND MED_ORG_DEPT_NM LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员姓名）在医院（医疗机构代码）中就诊科室名称包含（部分科室名称）的所有医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM t_kc21 WHERE PERSON_NM = $1 AND MED_SER_ORG_NO = $2 AND MED_ORG_DEPT_NM LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某医院在某段时间内所有某姓患者的医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医院（医疗机构代码）在（时间段）内所有姓（人员姓）的患者的医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3 AND PERSON_NM LIKE $4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>警察</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某患者在某医院入院诊断疾病名称包含某关键字的医疗就诊记录编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员ID）在医院（医疗机构代码）入院诊断疾病名称包含（部分疾病名称）的医疗就诊记录编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_ID = $1 AND MED_SER_ORG_NO = $2 AND IN_DIAG_DIS_NM LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员姓名）在医院（医疗机构代码）入院诊断疾病名称包含（部分疾病名称）的医疗就诊记录编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_NM = $1 AND MED_SER_ORG_NO = $2 AND IN_DIAG_DIS_NM LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某患者在某医院出院诊断疾病名称包含某关键字的医疗就诊记录编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某患者在某医院出院诊断疾病名称包含某关键字的医疗就诊记录编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员ID）在医院（医疗机构代码）出院诊断疾病名称包含（部分疾病名称）的医疗就诊记录编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员姓名）在医院（医疗机构代码）出院诊断疾病名称包含（部分疾病名称）的医疗就诊记录编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_ID = $1 AND MED_SER_ORG_NO = $2 AND OUT_DIAG_DIS_NM LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_NM = $1 AND MED_SER_ORG_NO = $2 AND OUT_DIAG_DIS_NM LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某患者在某医院的某次出院诊断结果，其中出院诊断医生为某姓</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员ID）在医院（医疗机构代码）的某次出院诊断结果，其中出院诊断医生姓（人员姓）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT OUT_DIAG_DIS_CD, OUT_DIAG_DIS_NM FROM t_kc21 WHERE PERSON_ID = $1 AND MED_SER_ORG_NO = $2 AND OUT_DIAG_DOC_NM LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>警察</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员姓名）在医院（医疗机构代码）的某次出院诊断结果，其中出院诊断医生姓（人员姓）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT OUT_DIAG_DIS_CD, OUT_DIAG_DIS_NM FROM t_kc21 WHERE PERSON_NM = $1 AND MED_SER_ORG_NO = $2 AND OUT_DIAG_DOC_NM LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某次医疗就诊中开出的所有名称包含某关键字的药品及其金额</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医疗就诊（医疗就诊ID）中开出的所有名称包含（部分社保三大目录名称）的药品及其金额</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM, AMOUNT FROM t_kc22 WHERE MED_CLINIC_ID = $1 AND SOC_SRT_DIRE_NM LIKE $2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中就诊科室名称不包含某关键字的所有医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中就诊科室名称不包含某关键字的所有医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员ID）在医院（医疗机构代码）中就诊科室名称不包含（部分科室名称）的所有医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员姓名）在医院（医疗机构代码）中就诊科室名称不包含（部分科室名称）的所有医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM t_kc21 WHERE PERSON_ID = $1 AND MED_SER_ORG_NO = $2 AND MED_ORG_DEPT_NM NOT LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM t_kc21 WHERE PERSON_NM = $1 AND MED_SER_ORG_NO = $2 AND MED_ORG_DEPT_NM NOT LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某患者在某医院入院诊断疾病名称不包含某关键字的医疗就诊记录编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某患者在某医院入院诊断疾病名称不包含某关键字的医疗就诊记录编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某患者在某医院出院诊断疾病名称不包含某关键字的医疗就诊记录编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员ID）在医院（医疗机构代码）入院诊断疾病名称不包含（部分疾病名称）的医疗就诊记录编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员姓名）在医院（医疗机构代码）入院诊断疾病名称不包含（部分疾病名称）的医疗就诊记录编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员ID）在医院（医疗机构代码）出院诊断疾病名称不包含（部分疾病名称）的医疗就诊记录编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员姓名）在医院（医疗机构代码）出院诊断疾病名称不包含（部分疾病名称）的医疗就诊记录编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_ID = $1 AND MED_SER_ORG_NO = $2 AND IN_DIAG_DIS_NM NOT LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_NM = $1 AND MED_SER_ORG_NO = $2 AND IN_DIAG_DIS_NM NOT LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_ID = $1 AND MED_SER_ORG_NO = $2 AND OUT_DIAG_DIS_NM NOT LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_NM = $1 AND MED_SER_ORG_NO = $2 AND OUT_DIAG_DIS_NM NOT LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某次医疗就诊中开出的所有名称不包含某关键字的药品及其金额</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医疗就诊（医疗就诊ID）中开出的所有名称不包含（部分社保三大目录名称）的药品及其金额</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM, AMOUNT FROM t_kc22 WHERE MED_CLINIC_ID = $1 AND SOC_SRT_DIRE_NM NOT LIKE $2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某次医疗就诊中名称包含某关键字的科室开出的所有医疗费用明细项目</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医疗就诊（医疗就诊ID）中名称包含（部分科室名称）的科室开出的所有医疗费用明细项目</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM t_kc22 WHERE MED_CLINIC_ID = $1 AND MED_ORG_DEPT_NM LIKE $2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某次医疗就诊中名称不包含某关键字的科室开出的所有医疗费用明细项目</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医疗就诊（医疗就诊ID）中名称不包含（部分科室名称）的科室开出的所有医疗费用明细项目</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM t_kc22 WHERE MED_CLINIC_ID = $1 AND MED_ORG_DEPT_NM NOT LIKE $2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某次医疗就诊中某姓医师开具的所有药品</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医疗就诊（医疗就诊ID）中姓（人员姓）的医师开具的所有药品</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM FROM t_kc22 WHERE MED_CLINIC_ID = $1 AND HOSP_DOC_NM LIKE $2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某次医疗就诊中名称包含某关键字的科室开出的所有检验报告单的编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医疗就诊（门诊就诊流水号或住院就诊流水号）中名称包含（部分科室名称）的科室开出的所有检验报告单的编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT BGDH FROM jybgb WHERE JZLSH = $1 AND KSMC LIKE $2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医生</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某次医疗就诊中名称不包含某关键字的科室开出的所有检验报告单的编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医疗就诊（门诊就诊流水号或住院就诊流水号）中名称不包含（部分科室名称）的科室开出的所有检验报告单的编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT BGDH FROM jybgb WHERE JZLSH = $1 AND KSMC NOT LIKE $2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医疗就诊（门诊就诊流水号或住院就诊流水号）中姓（人员姓）的检测人负责的所有检测指标名称及其结果定量与结果定量单位</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某次医疗就诊中某姓检测人负责的所有检测指标名称及其结果定量与结果定量单位</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT jyjgzbb.JCZBMC, jyjgzbb.JCZBJGDL, jyjgzbb.JCZBJGDW FROM jybgb JOIN jyjgzbb ON jybgb.YLJGDM = jyjgzbb.YLJGDM AND jybgb.BGDH = jyjgzbb.BGDH WHERE jybgb.JZLSH = $1 AND jyjgzbb.JCRXM LIKE $2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>警察</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中就诊科室名称包含某关键字的所有门诊就诊记录的流水号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员ID）在医院（医疗机构代码）中就诊科室名称包含（部分科室名称）的所有门诊就诊记录的流水号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医生</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员姓名）在医院（医疗机构代码）中就诊科室名称包含（部分科室名称）的所有门诊就诊记录的流水号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT mzjzjlb.JZLSH FROM person_info JOIN hz_info JOIN mzjzjlb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX WHERE person_info.XM = $1 AND hz_info.YLJGDM = $2 AND mzjzjlb.JZKSMC LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中门诊诊断名称包含某关键字的门诊就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员ID）在医院（医疗机构代码）中门诊诊断名称包含（部分疾病名称）的门诊就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT mzjzjlb.JZLSH FROM hz_info JOIN mzjzjlb ON hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX WHERE hz_info.RYBH = $1 AND hz_info.YLJGDM = $2 AND mzjzjlb.JZKSMC LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT mzjzjlb.* FROM hz_info JOIN mzjzjlb ON hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX WHERE hz_info.RYBH = $1 AND hz_info.YLJGDM = $2 AND mzjzjlb.JZZDSM LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医生</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员姓名）在医院（医疗机构代码）中门诊诊断名称包含（部分疾病名称）的门诊就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中就诊科室名称不包含某关键字的所有门诊就诊记录的流水号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中就诊科室名称不包含某关键字的所有门诊就诊记录的流水号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员ID）在医院（医疗机构代码）中就诊科室名称不包含（部分科室名称）的所有门诊就诊记录的流水号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员姓名）在医院（医疗机构代码）中就诊科室名称不包含（部分科室名称）的所有门诊就诊记录的流水号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT mzjzjlb.JZLSH FROM hz_info JOIN mzjzjlb ON hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX WHERE hz_info.RYBH = $1 AND hz_info.YLJGDM = $2 AND mzjzjlb.JZKSMC NOT LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT mzjzjlb.JZLSH FROM person_info JOIN hz_info JOIN mzjzjlb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX WHERE person_info.XM = $1 AND hz_info.YLJGDM = $2 AND mzjzjlb.JZKSMC NOT LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中门诊诊断名称不包含某关键字的门诊就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中门诊诊断名称不包含某关键字的门诊就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员ID）在医院（医疗机构代码）中门诊诊断名称不包含（部分疾病名称）的门诊就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员姓名）在医院（医疗机构代码）中门诊诊断名称不包含（部分疾病名称）的门诊就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT mzjzjlb.* FROM hz_info JOIN mzjzjlb ON hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX WHERE hz_info.RYBH = $1 AND hz_info.YLJGDM = $2 AND mzjzjlb.JZZDSM NOT LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT mzjzjlb.* FROM person_info JOIN hz_info JOIN mzjzjlb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX WHERE person_info.XM = $1 AND hz_info.YLJGDM = $2 AND mzjzjlb.JZZDSM LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT mzjzjlb.* FROM person_info JOIN hz_info JOIN mzjzjlb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX WHERE person_info.XM = $1 AND hz_info.YLJGDM = $2 AND mzjzjlb.JZZDSM NOT LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中入院科室名称包含某关键字的住院就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员ID）在医院（医疗机构代码）中入院科室名称包含（部分科室名称）的住院就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT zyjzjlb.* FROM hz_info JOIN zyjzjlb ON hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX WHERE hz_info.RYBH = $1 AND hz_info.YLJGDM = $2 AND zyjzjlb.JZKSMC LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医生</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中入院科室名称不包含某关键字的住院就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中入院科室名称不包含某关键字的住院就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员姓名）在医院（医疗机构代码）中入院科室名称包含（部分科室名称）的住院就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员姓名）在医院（医疗机构代码）中入院科室名称不包含（部分科室名称）的住院就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员ID）在医院（医疗机构代码）中入院科室名称不包含（部分科室名称）的住院就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT zyjzjlb.* FROM hz_info JOIN zyjzjlb ON hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX WHERE hz_info.RYBH = $1 AND hz_info.YLJGDM = $2 AND zyjzjlb.JZKSMC NOT LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT zyjzjlb.* FROM person_info JOIN hz_info JOIN zyjzjlb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX WHERE person_info.XM = $1 AND hz_info.YLJGDM = $2 AND zyjzjlb.JZKSMC LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT zyjzjlb.* FROM person_info JOIN hz_info JOIN zyjzjlb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX WHERE person_info.XM = $1 AND hz_info.YLJGDM = $2 AND zyjzjlb.JZKSMC NOT LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员ID）在医院（医疗机构代码）中出院科室名称包含（部分科室名称）的住院就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员姓名）在医院（医疗机构代码）中出院科室名称包含（部分科室名称）的住院就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员ID）在医院（医疗机构代码）中出院科室名称不包含（部分科室名称）的住院就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员姓名）在医院（医疗机构代码）中出院科室名称不包含（部分科室名称）的住院就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中出院科室名称包含某关键字的住院就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中出院科室名称不包含某关键字的住院就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中出院科室名称不包含某关键字的住院就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT zyjzjlb.* FROM hz_info JOIN zyjzjlb ON hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX WHERE hz_info.RYBH = $1 AND hz_info.YLJGDM = $2 AND zyjzjlb.CYKSMC LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT zyjzjlb.* FROM person_info JOIN hz_info JOIN zyjzjlb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX WHERE person_info.XM = $1 AND hz_info.YLJGDM = $2 AND zyjzjlb.CYKSMC LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT zyjzjlb.* FROM hz_info JOIN zyjzjlb ON hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX WHERE hz_info.RYBH = $1 AND hz_info.YLJGDM = $2 AND zyjzjlb.CYKSMC NOT LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT zyjzjlb.* FROM person_info JOIN hz_info JOIN zyjzjlb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX WHERE person_info.XM = $1 AND hz_info.YLJGDM = $2 AND zyjzjlb.CYKSMC NOT LIKE $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者在某医院中在某时间段内被开出的所有药品编码和名称</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员ID）在医院（医疗机构代码）中在（时间段）内被开出的所有药品编码和名称</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM FROM t_kc22 WHERE MED_CLINIC_ID IN (SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_ID = $1 AND MED_SER_ORG_NO = $2 AND IN_HOSP_DATE BETWEEN $3 AND $4)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出患者（人员姓名）在医院（医疗机构代码）中在（时间段）内被开出的所有药品编码和名称</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM FROM t_kc22 WHERE MED_CLINIC_ID IN (SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_NM = $1 AND MED_SER_ORG_NO = $2 AND IN_HOSP_DATE BETWEEN $3 AND $4)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者在某医院中被开出的单价最高的药品编码和名称及其单价</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员ID）在医院（医疗机构代码）中被开出的单价最高的药品编码和名称及其单价</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM, UNIVALENT FROM t_kc22 WHERE MED_CLINIC_ID IN (SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_ID = $1 AND MED_SER_ORG_NO = $2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员姓名）在医院（医疗机构代码）中被开出的单价最高的药品编码和名称及其单价</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM, UNIVALENT FROM t_kc22 WHERE MED_CLINIC_ID IN (SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_NM = $1 AND MED_SER_ORG_NO = $2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者不在某医院中被开出的单价最高的药品编码和名称及其单价</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者不在某医院中被开出的单价最高的药品编码和名称及其单价</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员ID）不在医院（医疗机构代码）中被开出的单价最高的药品编码和名称及其单价</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员姓名）不在医院（医疗机构代码）中被开出的单价最高的药品编码和名称及其单价</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM, UNIVALENT FROM t_kc22 WHERE MED_CLINIC_ID NOT IN (SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_ID = $1 AND MED_SER_ORG_NO = $2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM, UNIVALENT FROM t_kc22 WHERE MED_CLINIC_ID NOT IN (SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_NM = $1 AND MED_SER_ORG_NO = $2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者在哪几家医院被开出过某药品</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员ID）在哪几家医院被开出过药品（社保三大目录统一编码）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_SER_ORG_NO FROM t_kc21 WHERE PERSON_ID = $1 AND MED_CLINIC_ID IN (SELECT MED_CLINIC_ID FROM t_kc22 WHERE SOC_SRT_DIRE_CD = $2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>警察</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员ID）在哪几家医院被开出过（社保三大目录名称）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员姓名）在哪几家医院被开出过药品（社保三大目录统一编码）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员姓名）在哪几家医院被开出过药品（社保三大目录名称）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_SER_ORG_NO FROM t_kc21 WHERE PERSON_ID = $1 AND MED_CLINIC_ID IN (SELECT MED_CLINIC_ID FROM t_kc22 WHERE SOC_SRT_DIRE_NM = $2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_SER_ORG_NO FROM t_kc21 WHERE PERSON_NM = $1 AND MED_CLINIC_ID IN (SELECT MED_CLINIC_ID FROM t_kc22 WHERE SOC_SRT_DIRE_CD = $2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_SER_ORG_NO FROM t_kc21 WHERE PERSON_NM = $1 AND MED_CLINIC_ID IN (SELECT MED_CLINIC_ID FROM t_kc22 WHERE SOC_SRT_DIRE_NM = $2)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2496,7 +3176,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2817,17 +3497,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB327"/>
+  <dimension ref="A1:AB361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C169" workbookViewId="0">
-      <selection activeCell="C187" sqref="C187"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="101" customWidth="1"/>
-    <col min="2" max="2" width="119" customWidth="1"/>
-    <col min="3" max="3" width="255" customWidth="1"/>
+    <col min="2" max="2" width="110.6640625" customWidth="1"/>
+    <col min="3" max="3" width="255.77734375" customWidth="1"/>
     <col min="4" max="28" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16438,13 +17116,27 @@
       <c r="AB312" s="3"/>
     </row>
     <row r="313" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A313" s="3"/>
-      <c r="B313" s="3"/>
-      <c r="C313" s="3"/>
-      <c r="D313" s="5"/>
-      <c r="E313" s="5"/>
-      <c r="F313" s="5"/>
-      <c r="G313" s="5"/>
+      <c r="A313" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D313" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="E313" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="F313" s="5">
+        <v>7</v>
+      </c>
+      <c r="G313" s="5" t="s">
+        <v>807</v>
+      </c>
       <c r="H313" s="3"/>
       <c r="I313" s="3"/>
       <c r="J313" s="3"/>
@@ -16468,13 +17160,27 @@
       <c r="AB313" s="3"/>
     </row>
     <row r="314" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A314" s="3"/>
-      <c r="B314" s="3"/>
-      <c r="C314" s="3"/>
-      <c r="D314" s="5"/>
-      <c r="E314" s="5"/>
-      <c r="F314" s="5"/>
-      <c r="G314" s="5"/>
+      <c r="A314" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="D314" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="E314" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="F314" s="5">
+        <v>7</v>
+      </c>
+      <c r="G314" s="5" t="s">
+        <v>807</v>
+      </c>
       <c r="H314" s="3"/>
       <c r="I314" s="3"/>
       <c r="J314" s="3"/>
@@ -16498,13 +17204,27 @@
       <c r="AB314" s="3"/>
     </row>
     <row r="315" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A315" s="3"/>
-      <c r="B315" s="3"/>
-      <c r="C315" s="3"/>
-      <c r="D315" s="5"/>
-      <c r="E315" s="5"/>
-      <c r="F315" s="5"/>
-      <c r="G315" s="5"/>
+      <c r="A315" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="D315" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="E315" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="F315" s="5">
+        <v>7</v>
+      </c>
+      <c r="G315" s="5" t="s">
+        <v>807</v>
+      </c>
       <c r="H315" s="3"/>
       <c r="I315" s="3"/>
       <c r="J315" s="3"/>
@@ -16528,13 +17248,27 @@
       <c r="AB315" s="3"/>
     </row>
     <row r="316" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A316" s="3"/>
-      <c r="B316" s="3"/>
-      <c r="C316" s="3"/>
-      <c r="D316" s="5"/>
-      <c r="E316" s="5"/>
-      <c r="F316" s="5"/>
-      <c r="G316" s="5"/>
+      <c r="A316" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="D316" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="E316" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="F316" s="5">
+        <v>7</v>
+      </c>
+      <c r="G316" s="5" t="s">
+        <v>807</v>
+      </c>
       <c r="H316" s="3"/>
       <c r="I316" s="3"/>
       <c r="J316" s="3"/>
@@ -16558,13 +17292,27 @@
       <c r="AB316" s="3"/>
     </row>
     <row r="317" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A317" s="3"/>
-      <c r="B317" s="3"/>
-      <c r="C317" s="3"/>
-      <c r="D317" s="5"/>
-      <c r="E317" s="5"/>
-      <c r="F317" s="5"/>
-      <c r="G317" s="5"/>
+      <c r="A317" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="D317" s="5" t="s">
+        <v>813</v>
+      </c>
+      <c r="E317" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="F317" s="5">
+        <v>5</v>
+      </c>
+      <c r="G317" s="5" t="s">
+        <v>815</v>
+      </c>
       <c r="H317" s="3"/>
       <c r="I317" s="3"/>
       <c r="J317" s="3"/>
@@ -16588,13 +17336,27 @@
       <c r="AB317" s="3"/>
     </row>
     <row r="318" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A318" s="3"/>
-      <c r="B318" s="3"/>
-      <c r="C318" s="3"/>
-      <c r="D318" s="5"/>
-      <c r="E318" s="5"/>
-      <c r="F318" s="5"/>
-      <c r="G318" s="5"/>
+      <c r="A318" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="D318" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="E318" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="F318" s="5">
+        <v>7</v>
+      </c>
+      <c r="G318" s="5" t="s">
+        <v>821</v>
+      </c>
       <c r="H318" s="3"/>
       <c r="I318" s="3"/>
       <c r="J318" s="3"/>
@@ -16618,13 +17380,27 @@
       <c r="AB318" s="3"/>
     </row>
     <row r="319" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A319" s="3"/>
-      <c r="B319" s="3"/>
-      <c r="C319" s="3"/>
-      <c r="D319" s="5"/>
-      <c r="E319" s="5"/>
-      <c r="F319" s="5"/>
-      <c r="G319" s="5"/>
+      <c r="A319" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="D319" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="E319" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="F319" s="5">
+        <v>7</v>
+      </c>
+      <c r="G319" s="5" t="s">
+        <v>821</v>
+      </c>
       <c r="H319" s="3"/>
       <c r="I319" s="3"/>
       <c r="J319" s="3"/>
@@ -16648,13 +17424,27 @@
       <c r="AB319" s="3"/>
     </row>
     <row r="320" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A320" s="3"/>
-      <c r="B320" s="3"/>
-      <c r="C320" s="3"/>
-      <c r="D320" s="5"/>
-      <c r="E320" s="5"/>
-      <c r="F320" s="5"/>
-      <c r="G320" s="5"/>
+      <c r="A320" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="D320" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="E320" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="F320" s="5">
+        <v>7</v>
+      </c>
+      <c r="G320" s="5" t="s">
+        <v>821</v>
+      </c>
       <c r="H320" s="3"/>
       <c r="I320" s="3"/>
       <c r="J320" s="3"/>
@@ -16678,13 +17468,27 @@
       <c r="AB320" s="3"/>
     </row>
     <row r="321" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A321" s="3"/>
-      <c r="B321" s="3"/>
-      <c r="C321" s="3"/>
-      <c r="D321" s="5"/>
-      <c r="E321" s="5"/>
-      <c r="F321" s="5"/>
-      <c r="G321" s="5"/>
+      <c r="A321" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="D321" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="E321" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="F321" s="5">
+        <v>7</v>
+      </c>
+      <c r="G321" s="5" t="s">
+        <v>821</v>
+      </c>
       <c r="H321" s="3"/>
       <c r="I321" s="3"/>
       <c r="J321" s="3"/>
@@ -16708,13 +17512,27 @@
       <c r="AB321" s="3"/>
     </row>
     <row r="322" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A322" s="3"/>
-      <c r="B322" s="3"/>
-      <c r="C322" s="3"/>
-      <c r="D322" s="5"/>
-      <c r="E322" s="5"/>
-      <c r="F322" s="5"/>
-      <c r="G322" s="5"/>
+      <c r="A322" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="D322" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="E322" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="F322" s="5">
+        <v>7</v>
+      </c>
+      <c r="G322" s="5" t="s">
+        <v>821</v>
+      </c>
       <c r="H322" s="3"/>
       <c r="I322" s="3"/>
       <c r="J322" s="3"/>
@@ -16738,13 +17556,27 @@
       <c r="AB322" s="3"/>
     </row>
     <row r="323" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A323" s="3"/>
-      <c r="B323" s="3"/>
-      <c r="C323" s="3"/>
-      <c r="D323" s="5"/>
-      <c r="E323" s="5"/>
-      <c r="F323" s="5"/>
-      <c r="G323" s="5"/>
+      <c r="A323" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="D323" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="E323" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="F323" s="5">
+        <v>7</v>
+      </c>
+      <c r="G323" s="5" t="s">
+        <v>821</v>
+      </c>
       <c r="H323" s="3"/>
       <c r="I323" s="3"/>
       <c r="J323" s="3"/>
@@ -16768,13 +17600,27 @@
       <c r="AB323" s="3"/>
     </row>
     <row r="324" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A324" s="3"/>
-      <c r="B324" s="3"/>
-      <c r="C324" s="3"/>
-      <c r="D324" s="5"/>
-      <c r="E324" s="5"/>
-      <c r="F324" s="5"/>
-      <c r="G324" s="5"/>
+      <c r="A324" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="D324" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="E324" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="F324" s="5">
+        <v>7</v>
+      </c>
+      <c r="G324" s="5" t="s">
+        <v>821</v>
+      </c>
       <c r="H324" s="3"/>
       <c r="I324" s="3"/>
       <c r="J324" s="3"/>
@@ -16798,13 +17644,27 @@
       <c r="AB324" s="3"/>
     </row>
     <row r="325" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A325" s="3"/>
-      <c r="B325" s="3"/>
-      <c r="C325" s="3"/>
-      <c r="D325" s="5"/>
-      <c r="E325" s="5"/>
-      <c r="F325" s="5"/>
-      <c r="G325" s="5"/>
+      <c r="A325" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="D325" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="E325" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="F325" s="5">
+        <v>7</v>
+      </c>
+      <c r="G325" s="5" t="s">
+        <v>821</v>
+      </c>
       <c r="H325" s="3"/>
       <c r="I325" s="3"/>
       <c r="J325" s="3"/>
@@ -16828,13 +17688,27 @@
       <c r="AB325" s="3"/>
     </row>
     <row r="326" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A326" s="3"/>
-      <c r="B326" s="3"/>
-      <c r="C326" s="3"/>
-      <c r="D326" s="5"/>
-      <c r="E326" s="5"/>
-      <c r="F326" s="5"/>
-      <c r="G326" s="5"/>
+      <c r="A326" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="D326" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="E326" s="5" t="s">
+        <v>834</v>
+      </c>
+      <c r="F326" s="5">
+        <v>5</v>
+      </c>
+      <c r="G326" s="5" t="s">
+        <v>835</v>
+      </c>
       <c r="H326" s="3"/>
       <c r="I326" s="3"/>
       <c r="J326" s="3"/>
@@ -16858,13 +17732,27 @@
       <c r="AB326" s="3"/>
     </row>
     <row r="327" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A327" s="3"/>
-      <c r="B327" s="3"/>
-      <c r="C327" s="3"/>
-      <c r="D327" s="5"/>
-      <c r="E327" s="5"/>
-      <c r="F327" s="5"/>
-      <c r="G327" s="5"/>
+      <c r="A327" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="D327" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="E327" s="5" t="s">
+        <v>834</v>
+      </c>
+      <c r="F327" s="5">
+        <v>5</v>
+      </c>
+      <c r="G327" s="5" t="s">
+        <v>835</v>
+      </c>
       <c r="H327" s="3"/>
       <c r="I327" s="3"/>
       <c r="J327" s="3"/>
@@ -16887,6 +17775,914 @@
       <c r="AA327" s="3"/>
       <c r="AB327" s="3"/>
     </row>
+    <row r="328" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A328" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="D328" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="E328" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="F328" s="5">
+        <v>8</v>
+      </c>
+      <c r="G328" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="H328" s="3"/>
+      <c r="I328" s="3"/>
+      <c r="J328" s="3"/>
+      <c r="K328" s="3"/>
+      <c r="L328" s="3"/>
+      <c r="M328" s="3"/>
+      <c r="N328" s="3"/>
+      <c r="O328" s="3"/>
+      <c r="P328" s="3"/>
+      <c r="Q328" s="3"/>
+      <c r="R328" s="3"/>
+      <c r="S328" s="3"/>
+      <c r="T328" s="3"/>
+      <c r="U328" s="3"/>
+      <c r="V328" s="3"/>
+      <c r="W328" s="3"/>
+      <c r="X328" s="3"/>
+      <c r="Y328" s="3"/>
+      <c r="Z328" s="3"/>
+      <c r="AA328" s="3"/>
+      <c r="AB328" s="3"/>
+    </row>
+    <row r="329" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A329" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="D329" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="E329" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="F329" s="5">
+        <v>8</v>
+      </c>
+      <c r="G329" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="H329" s="3"/>
+      <c r="I329" s="3"/>
+      <c r="J329" s="3"/>
+      <c r="K329" s="3"/>
+      <c r="L329" s="3"/>
+      <c r="M329" s="3"/>
+      <c r="N329" s="3"/>
+      <c r="O329" s="3"/>
+      <c r="P329" s="3"/>
+      <c r="Q329" s="3"/>
+      <c r="R329" s="3"/>
+      <c r="S329" s="3"/>
+      <c r="T329" s="3"/>
+      <c r="U329" s="3"/>
+      <c r="V329" s="3"/>
+      <c r="W329" s="3"/>
+      <c r="X329" s="3"/>
+      <c r="Y329" s="3"/>
+      <c r="Z329" s="3"/>
+      <c r="AA329" s="3"/>
+      <c r="AB329" s="3"/>
+    </row>
+    <row r="330" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A330" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="D330" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="E330" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="F330" s="5">
+        <v>8</v>
+      </c>
+      <c r="G330" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="H330" s="3"/>
+      <c r="I330" s="3"/>
+      <c r="J330" s="3"/>
+      <c r="K330" s="3"/>
+      <c r="L330" s="3"/>
+      <c r="M330" s="3"/>
+      <c r="N330" s="3"/>
+      <c r="O330" s="3"/>
+      <c r="P330" s="3"/>
+      <c r="Q330" s="3"/>
+      <c r="R330" s="3"/>
+      <c r="S330" s="3"/>
+      <c r="T330" s="3"/>
+      <c r="U330" s="3"/>
+      <c r="V330" s="3"/>
+      <c r="W330" s="3"/>
+      <c r="X330" s="3"/>
+      <c r="Y330" s="3"/>
+      <c r="Z330" s="3"/>
+      <c r="AA330" s="3"/>
+      <c r="AB330" s="3"/>
+    </row>
+    <row r="331" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A331" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="D331" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="E331" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="F331" s="5">
+        <v>8</v>
+      </c>
+      <c r="G331" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="H331" s="3"/>
+      <c r="I331" s="3"/>
+      <c r="J331" s="3"/>
+      <c r="K331" s="3"/>
+      <c r="L331" s="3"/>
+      <c r="M331" s="3"/>
+      <c r="N331" s="3"/>
+      <c r="O331" s="3"/>
+      <c r="P331" s="3"/>
+      <c r="Q331" s="3"/>
+      <c r="R331" s="3"/>
+      <c r="S331" s="3"/>
+      <c r="T331" s="3"/>
+      <c r="U331" s="3"/>
+      <c r="V331" s="3"/>
+      <c r="W331" s="3"/>
+      <c r="X331" s="3"/>
+      <c r="Y331" s="3"/>
+      <c r="Z331" s="3"/>
+      <c r="AA331" s="3"/>
+      <c r="AB331" s="3"/>
+    </row>
+    <row r="332" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A332" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="D332" s="5" t="s">
+        <v>873</v>
+      </c>
+      <c r="E332" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="F332" s="5">
+        <v>8</v>
+      </c>
+      <c r="G332" s="5" t="s">
+        <v>835</v>
+      </c>
+      <c r="H332" s="3"/>
+      <c r="I332" s="3"/>
+      <c r="J332" s="3"/>
+      <c r="K332" s="3"/>
+      <c r="L332" s="3"/>
+      <c r="M332" s="3"/>
+      <c r="N332" s="3"/>
+      <c r="O332" s="3"/>
+      <c r="P332" s="3"/>
+      <c r="Q332" s="3"/>
+      <c r="R332" s="3"/>
+      <c r="S332" s="3"/>
+      <c r="T332" s="3"/>
+      <c r="U332" s="3"/>
+      <c r="V332" s="3"/>
+      <c r="W332" s="3"/>
+      <c r="X332" s="3"/>
+      <c r="Y332" s="3"/>
+      <c r="Z332" s="3"/>
+      <c r="AA332" s="3"/>
+      <c r="AB332" s="3"/>
+    </row>
+    <row r="333" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A333" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="D333" s="5" t="s">
+        <v>877</v>
+      </c>
+      <c r="E333" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="F333" s="5">
+        <v>2</v>
+      </c>
+      <c r="G333" s="5" t="s">
+        <v>835</v>
+      </c>
+      <c r="H333" s="3"/>
+      <c r="I333" s="3"/>
+      <c r="J333" s="3"/>
+      <c r="K333" s="3"/>
+      <c r="L333" s="3"/>
+      <c r="M333" s="3"/>
+      <c r="N333" s="3"/>
+      <c r="O333" s="3"/>
+      <c r="P333" s="3"/>
+      <c r="Q333" s="3"/>
+      <c r="R333" s="3"/>
+      <c r="S333" s="3"/>
+      <c r="T333" s="3"/>
+      <c r="U333" s="3"/>
+      <c r="V333" s="3"/>
+      <c r="W333" s="3"/>
+      <c r="X333" s="3"/>
+      <c r="Y333" s="3"/>
+      <c r="Z333" s="3"/>
+      <c r="AA333" s="3"/>
+      <c r="AB333" s="3"/>
+    </row>
+    <row r="334" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A334" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="D334" s="5" t="s">
+        <v>877</v>
+      </c>
+      <c r="E334" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="F334" s="5">
+        <v>2</v>
+      </c>
+      <c r="G334" s="5" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="335" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A335" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="D335" s="5" t="s">
+        <v>885</v>
+      </c>
+      <c r="E335" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="F335" s="5">
+        <v>5</v>
+      </c>
+      <c r="G335" s="5" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="336" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A336" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="D336" s="5" t="s">
+        <v>890</v>
+      </c>
+      <c r="E336" s="5" t="s">
+        <v>891</v>
+      </c>
+      <c r="F336" s="5">
+        <v>2</v>
+      </c>
+      <c r="G336" s="5" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A337" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="D337" s="5" t="s">
+        <v>890</v>
+      </c>
+      <c r="E337" s="5" t="s">
+        <v>891</v>
+      </c>
+      <c r="F337" s="5">
+        <v>2</v>
+      </c>
+      <c r="G337" s="5" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A338" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="D338" s="5" t="s">
+        <v>890</v>
+      </c>
+      <c r="E338" s="5" t="s">
+        <v>891</v>
+      </c>
+      <c r="F338" s="5">
+        <v>2</v>
+      </c>
+      <c r="G338" s="5" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A339" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="D339" s="5" t="s">
+        <v>890</v>
+      </c>
+      <c r="E339" s="5" t="s">
+        <v>891</v>
+      </c>
+      <c r="F339" s="5">
+        <v>2</v>
+      </c>
+      <c r="G339" s="5" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A340" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="D340" s="5" t="s">
+        <v>899</v>
+      </c>
+      <c r="E340" s="5" t="s">
+        <v>900</v>
+      </c>
+      <c r="F340" s="5">
+        <v>2</v>
+      </c>
+      <c r="G340" s="5" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A341" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="D341" s="5" t="s">
+        <v>899</v>
+      </c>
+      <c r="E341" s="5" t="s">
+        <v>900</v>
+      </c>
+      <c r="F341" s="5">
+        <v>2</v>
+      </c>
+      <c r="G341" s="5" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A342" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="D342" s="5" t="s">
+        <v>899</v>
+      </c>
+      <c r="E342" s="5" t="s">
+        <v>900</v>
+      </c>
+      <c r="F342" s="5">
+        <v>2</v>
+      </c>
+      <c r="G342" s="5" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A343" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="D343" s="5" t="s">
+        <v>899</v>
+      </c>
+      <c r="E343" s="5" t="s">
+        <v>900</v>
+      </c>
+      <c r="F343" s="5">
+        <v>2</v>
+      </c>
+      <c r="G343" s="5" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A344" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="D344" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="E344" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="F344" s="5">
+        <v>2</v>
+      </c>
+      <c r="G344" s="5" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A345" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="D345" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="E345" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="F345" s="5">
+        <v>2</v>
+      </c>
+      <c r="G345" s="5" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A346" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="D346" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="E346" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="F346" s="5">
+        <v>2</v>
+      </c>
+      <c r="G346" s="5" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A347" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="D347" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="E347" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="F347" s="5">
+        <v>2</v>
+      </c>
+      <c r="G347" s="5" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A348" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="D348" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="E348" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="F348" s="5">
+        <v>2</v>
+      </c>
+      <c r="G348" s="5" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A349" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="D349" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="E349" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="F349" s="5">
+        <v>2</v>
+      </c>
+      <c r="G349" s="5" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A350" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="D350" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="E350" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="F350" s="5">
+        <v>2</v>
+      </c>
+      <c r="G350" s="5" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A351" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C351" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="D351" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="E351" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="F351" s="5">
+        <v>2</v>
+      </c>
+      <c r="G351" s="5" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A352" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="D352" s="5" t="s">
+        <v>944</v>
+      </c>
+      <c r="E352" s="5" t="s">
+        <v>945</v>
+      </c>
+      <c r="F352" s="5">
+        <v>8</v>
+      </c>
+      <c r="G352" s="5" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="353" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A353" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="D353" s="5" t="s">
+        <v>944</v>
+      </c>
+      <c r="E353" s="5" t="s">
+        <v>945</v>
+      </c>
+      <c r="F353" s="5">
+        <v>8</v>
+      </c>
+      <c r="G353" s="5" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="354" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A354" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="D354" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="E354" s="5" t="s">
+        <v>952</v>
+      </c>
+      <c r="F354" s="5">
+        <v>8</v>
+      </c>
+      <c r="G354" s="5" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A355" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="D355" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="E355" s="5" t="s">
+        <v>952</v>
+      </c>
+      <c r="F355" s="5">
+        <v>8</v>
+      </c>
+      <c r="G355" s="5" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="356" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A356" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="D356" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="E356" s="5" t="s">
+        <v>952</v>
+      </c>
+      <c r="F356" s="5">
+        <v>8</v>
+      </c>
+      <c r="G356" s="5" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A357" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="D357" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="E357" s="5" t="s">
+        <v>952</v>
+      </c>
+      <c r="F357" s="5">
+        <v>8</v>
+      </c>
+      <c r="G357" s="5" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A358" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="D358" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="E358" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="F358" s="5">
+        <v>5</v>
+      </c>
+      <c r="G358" s="5" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A359" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="D359" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="E359" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="F359" s="5">
+        <v>5</v>
+      </c>
+      <c r="G359" s="5" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="360" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A360" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="D360" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="E360" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="F360" s="5">
+        <v>5</v>
+      </c>
+      <c r="G360" s="5" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A361" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="C361" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="D361" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="E361" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="F361" s="5">
+        <v>5</v>
+      </c>
+      <c r="G361" s="5" t="s">
+        <v>965</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: ylsql with in, like, from sql
</commit_message>
<xml_diff>
--- a/dataset/templates.xlsx
+++ b/dataset/templates.xlsx
@@ -3681,22 +3681,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>SELECT COUNT(*) FROM (SELECT * FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &lt;= $4)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT * FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &lt; $4)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT * FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &gt;= $4)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT * FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &gt; $4)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>某医院有多少科室的平均医疗住院时长超过一定天数</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -3705,10 +3689,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>SELECT COUNT(*) FROM (SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD HAVING AVG(IN_HOSP_DAYS) &gt; $2)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>医保</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -3733,14 +3713,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>SELECT COUNT(*) FROM (SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD HAVING MAX(IN_HOSP_DAYS) &lt; $2)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD HAVING MIN(IN_HOSP_DAYS) &gt; $2)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>某医院在某时间段内有多少科室在门诊就诊中开出超过一定数量的检验报告单</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -3777,19 +3749,47 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>SELECT COUNT(*) FROM (SELECT * FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &gt;= $4)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT * FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &lt; $4)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT * FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &lt;= $4)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT * FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &gt; $4)</t>
+    <t>SELECT COUNT(*) FROM (SELECT t_kc21.MED_ORG_DEPT_CD FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &gt; $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT t_kc21.MED_ORG_DEPT_CD FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &gt;= $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT t_kc21.MED_ORG_DEPT_CD FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &lt; $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT t_kc21.MED_ORG_DEPT_CD FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &lt;= $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT MED_ORG_DEPT_CD FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD HAVING AVG(IN_HOSP_DAYS) &gt; $2) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT MED_ORG_DEPT_CD FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD HAVING MAX(IN_HOSP_DAYS) &lt; $2) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT MED_ORG_DEPT_CD FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD HAVING MIN(IN_HOSP_DAYS) &gt; $2) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT jybgb.KSBM FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &gt; $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT jybgb.KSBM FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &gt;= $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT jybgb.KSBM FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &lt; $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT jybgb.KSBM FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &lt;= $4) as T</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4184,7 +4184,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB414"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C387" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C414" sqref="C414"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20342,7 +20344,7 @@
         <v>1104</v>
       </c>
       <c r="C404" s="1" t="s">
-        <v>1117</v>
+        <v>1131</v>
       </c>
       <c r="D404" s="5" t="s">
         <v>1105</v>
@@ -20365,7 +20367,7 @@
         <v>1111</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>1116</v>
+        <v>1132</v>
       </c>
       <c r="D405" s="5" t="s">
         <v>1105</v>
@@ -20388,7 +20390,7 @@
         <v>1112</v>
       </c>
       <c r="C406" s="1" t="s">
-        <v>1115</v>
+        <v>1133</v>
       </c>
       <c r="D406" s="5" t="s">
         <v>1105</v>
@@ -20411,7 +20413,7 @@
         <v>1113</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>1114</v>
+        <v>1134</v>
       </c>
       <c r="D407" s="5" t="s">
         <v>1105</v>
@@ -20428,88 +20430,88 @@
     </row>
     <row r="408" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="C408" s="1" t="s">
-        <v>1120</v>
+        <v>1135</v>
       </c>
       <c r="D408" s="5" t="s">
         <v>1044</v>
       </c>
       <c r="E408" s="5" t="s">
-        <v>1121</v>
+        <v>1116</v>
       </c>
       <c r="F408" s="5">
         <v>6</v>
       </c>
       <c r="G408" s="5" t="s">
-        <v>1122</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="409" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
-        <v>1123</v>
+        <v>1118</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>1125</v>
+        <v>1120</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>1127</v>
+        <v>1136</v>
       </c>
       <c r="D409" s="5" t="s">
         <v>1044</v>
       </c>
       <c r="E409" s="5" t="s">
-        <v>1121</v>
+        <v>1116</v>
       </c>
       <c r="F409" s="5">
         <v>6</v>
       </c>
       <c r="G409" s="5" t="s">
-        <v>1122</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="410" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
-        <v>1124</v>
+        <v>1119</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>1126</v>
+        <v>1121</v>
       </c>
       <c r="C410" s="1" t="s">
-        <v>1128</v>
+        <v>1137</v>
       </c>
       <c r="D410" s="5" t="s">
         <v>1044</v>
       </c>
       <c r="E410" s="5" t="s">
-        <v>1121</v>
+        <v>1116</v>
       </c>
       <c r="F410" s="5">
         <v>6</v>
       </c>
       <c r="G410" s="5" t="s">
-        <v>1122</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="411" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
-        <v>1129</v>
+        <v>1122</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>1130</v>
+        <v>1123</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>1141</v>
+        <v>1138</v>
       </c>
       <c r="D411" s="5" t="s">
         <v>1064</v>
       </c>
       <c r="E411" s="5" t="s">
-        <v>1131</v>
+        <v>1124</v>
       </c>
       <c r="F411" s="5">
         <v>4</v>
@@ -20520,19 +20522,19 @@
     </row>
     <row r="412" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
-        <v>1132</v>
+        <v>1125</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>1135</v>
+        <v>1128</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="D412" s="5" t="s">
         <v>1064</v>
       </c>
       <c r="E412" s="5" t="s">
-        <v>1131</v>
+        <v>1124</v>
       </c>
       <c r="F412" s="5">
         <v>4</v>
@@ -20543,19 +20545,19 @@
     </row>
     <row r="413" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
-        <v>1133</v>
+        <v>1126</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="C413" s="1" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="D413" s="5" t="s">
         <v>1064</v>
       </c>
       <c r="E413" s="5" t="s">
-        <v>1131</v>
+        <v>1124</v>
       </c>
       <c r="F413" s="5">
         <v>4</v>
@@ -20566,19 +20568,19 @@
     </row>
     <row r="414" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
-        <v>1134</v>
+        <v>1127</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>1137</v>
+        <v>1130</v>
       </c>
       <c r="C414" s="1" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="D414" s="5" t="s">
         <v>1064</v>
       </c>
       <c r="E414" s="5" t="s">
-        <v>1131</v>
+        <v>1124</v>
       </c>
       <c r="F414" s="5">
         <v>4</v>

</xml_diff>

<commit_message>
fix: check new templates
</commit_message>
<xml_diff>
--- a/dataset/templates.xlsx
+++ b/dataset/templates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2434" uniqueCount="1142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2422" uniqueCount="1136">
   <si>
     <t>一家医院调取患者之前在其他所有医院的就诊、检查数据，医保对可疑的就诊调取医院的就诊信息，与医保数据进行比对</t>
   </si>
@@ -3017,22 +3017,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>患者不在某医院中被开出的单价最高的药品编码和名称及其单价</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>患者不在某医院中被开出的单价最高的药品编码和名称及其单价</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>患者（人员ID）不在医院（医疗机构代码）中被开出的单价最高的药品编码和名称及其单价</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>患者（人员姓名）不在医院（医疗机构代码）中被开出的单价最高的药品编码和名称及其单价</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>患者在哪几家医院被开出过某药品</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -3085,14 +3069,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM, UNIVALENT FROM t_kc22 WHERE MED_CLINIC_ID NOT IN (SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_ID = $1 AND MED_SER_ORG_NO = $2) ORDER BY UNIVALENT DESC LIMIT 1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM, UNIVALENT FROM t_kc22 WHERE MED_CLINIC_ID NOT IN (SELECT MED_CLINIC_ID FROM t_kc21 WHERE PERSON_NM = $1 AND MED_SER_ORG_NO = $2) ORDER BY UNIVALENT DESC LIMIT 1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>患者在哪几次医疗记录中被开出过超过某金额的药品？列出医疗就诊编号</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -3597,199 +3573,199 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>医生</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员姓名）的哪些检验报告单对应的检验结果指标均正常？列出检验报告单号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(SELECT jybgb.BGDH FROM person_info JOIN hz_info JOIN mzjzjlb JOIN jybgb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX AND mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE person_info.XM = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &lt; CKZFWXX OR JCZBJGDL &gt; CKZFWSX)) UNION (SELECT jybgb.BGDH FROM person_info JOIN hz_info JOIN zyjzjlb JOIN jybgb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX AND zyjzjlb.YLJGDM = jybgb.YLJGDM AND zyjzjlb.JZLSH = jybgb.JZLSH WHERE person_info.XM = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &lt; CKZFWXX OR JCZBJGDL &gt; CKZFWSX))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者的哪些检验报告单对应的检验结果指标均异常？列出检验报告单号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者的哪些检验报告单对应的检验结果指标均异常？列出检验报告单号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员ID）的哪些检验报告单对应的检验结果指标均异常？列出检验报告单号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者（人员姓名）的哪些检验报告单对应的检验结果指标均异常？列出检验报告单号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(SELECT jybgb.BGDH FROM hz_info JOIN mzjzjlb JOIN jybgb ON hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX AND mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE hz_info.RYBH = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &gt;= CKZFWXX AND JCZBJGDL &lt;= CKZFWSX)) UNION (SELECT jybgb.BGDH FROM hz_info JOIN zyjzjlb JOIN jybgb ON hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX AND zyjzjlb.YLJGDM = jybgb.YLJGDM AND zyjzjlb.JZLSH = jybgb.JZLSH WHERE hz_info.RYBH = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &gt;= CKZFWXX AND JCZBJGDL &lt;= CKZFWSX))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(SELECT jybgb.BGDH FROM person_info JOIN hz_info JOIN mzjzjlb JOIN jybgb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX AND mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE person_info.XM = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &gt;= CKZFWXX AND JCZBJGDL &lt;= CKZFWSX)) UNION (SELECT jybgb.BGDH FROM person_info JOIN hz_info JOIN zyjzjlb JOIN jybgb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX AND zyjzjlb.YLJGDM = jybgb.YLJGDM AND zyjzjlb.JZLSH = jybgb.JZLSH WHERE person_info.XM = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &gt;= CKZFWXX AND JCZBJGDL &lt;= CKZFWSX))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院在某时间段内有多少科室涉及医疗费总额超过某金额</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）在（时间段）内有多少科室涉及医疗费总额超过（大实数）元</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院在某时间段内有多少科室涉及医疗费总额不低于某金额</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院在某时间段内有多少科室涉及医疗费总额低于某金额</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院在某时间段内有多少科室涉及医疗费总额不超过某金额</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）在（时间段）内有多少科室涉及医疗费总额不低于（大实数）元</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）在（时间段）内有多少科室涉及医疗费总额低于（大实数）元</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）在（时间段）内有多少科室涉及医疗费总额不超过（大实数）元</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院有多少科室的平均医疗住院时长超过一定天数</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）有多少科室的平均医疗住院时长超过（整数）天</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院有多少科室的最长医疗住院时长少于一定天数</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院有多少科室的最短医疗住院时长超过一定天数</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）有多少科室的最长医疗住院时长少于（整数）天</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）有多少科室的最短医疗住院时长超过（整数）天</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院在某时间段内有多少科室在门诊就诊中开出超过一定数量的检验报告单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）在（时间段）内有多少科室在门诊就诊中开出超过（整数）张检验报告单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院在某时间段内有多少科室在门诊就诊中开出不少于一定数量的检验报告单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院在某时间段内有多少科室在门诊就诊中开出少于一定数量的检验报告单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院在某时间段内有多少科室在门诊就诊中开出不超过一定数量的检验报告单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）在（时间段）内有多少科室在门诊就诊中开出不少于（整数）张检验报告单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）在（时间段）内有多少科室在门诊就诊中开出少于（整数）张检验报告单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）在（时间段）内有多少科室在门诊就诊中开出不超过（整数）张检验报告单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT t_kc21.MED_ORG_DEPT_CD FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &gt; $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT t_kc21.MED_ORG_DEPT_CD FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &gt;= $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT t_kc21.MED_ORG_DEPT_CD FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &lt; $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT t_kc21.MED_ORG_DEPT_CD FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &lt;= $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT MED_ORG_DEPT_CD FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD HAVING AVG(IN_HOSP_DAYS) &gt; $2) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT MED_ORG_DEPT_CD FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD HAVING MAX(IN_HOSP_DAYS) &lt; $2) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT MED_ORG_DEPT_CD FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD HAVING MIN(IN_HOSP_DAYS) &gt; $2) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT jybgb.KSBM FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &gt; $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT jybgb.KSBM FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &gt;= $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT jybgb.KSBM FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &lt; $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM (SELECT jybgb.KSBM FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &lt;= $4) as T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>(SELECT jybgb.BGDH FROM hz_info JOIN mzjzjlb JOIN jybgb ON hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX AND mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE hz_info.RYBH = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &lt; CKZFWXX OR JCZBJGDL &gt; CKZFWSX)) UNION (SELECT jybgb.BGDH FROM hz_info JOIN zyjzjlb JOIN jybgb ON hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX AND zyjzjlb.YLJGDM = jybgb.YLJGDM AND zyjzjlb.JZLSH = jybgb.JZLSH WHERE hz_info.RYBH = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &lt; CKZFWXX OR JCZBJGDL &gt; CKZFWSX))</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医生</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>患者（人员姓名）的哪些检验报告单对应的检验结果指标均正常？列出检验报告单号</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(SELECT jybgb.BGDH FROM person_info JOIN hz_info JOIN mzjzjlb JOIN jybgb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX AND mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE person_info.XM = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &lt; CKZFWXX OR JCZBJGDL &gt; CKZFWSX)) UNION (SELECT jybgb.BGDH FROM person_info JOIN hz_info JOIN zyjzjlb JOIN jybgb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX AND zyjzjlb.YLJGDM = jybgb.YLJGDM AND zyjzjlb.JZLSH = jybgb.JZLSH WHERE person_info.XM = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &lt; CKZFWXX OR JCZBJGDL &gt; CKZFWSX))</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>患者的哪些检验报告单对应的检验结果指标均异常？列出检验报告单号</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>患者的哪些检验报告单对应的检验结果指标均异常？列出检验报告单号</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>患者（人员ID）的哪些检验报告单对应的检验结果指标均异常？列出检验报告单号</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>患者（人员姓名）的哪些检验报告单对应的检验结果指标均异常？列出检验报告单号</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(SELECT jybgb.BGDH FROM hz_info JOIN mzjzjlb JOIN jybgb ON hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX AND mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE hz_info.RYBH = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &gt;= CKZFWXX AND JCZBJGDL &lt;= CKZFWSX)) UNION (SELECT jybgb.BGDH FROM hz_info JOIN zyjzjlb JOIN jybgb ON hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX AND zyjzjlb.YLJGDM = jybgb.YLJGDM AND zyjzjlb.JZLSH = jybgb.JZLSH WHERE hz_info.RYBH = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &gt;= CKZFWXX AND JCZBJGDL &lt;= CKZFWSX))</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(SELECT jybgb.BGDH FROM person_info JOIN hz_info JOIN mzjzjlb JOIN jybgb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX AND mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE person_info.XM = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &gt;= CKZFWXX AND JCZBJGDL &lt;= CKZFWSX)) UNION (SELECT jybgb.BGDH FROM person_info JOIN hz_info JOIN zyjzjlb JOIN jybgb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX AND zyjzjlb.YLJGDM = jybgb.YLJGDM AND zyjzjlb.JZLSH = jybgb.JZLSH WHERE person_info.XM = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &gt;= CKZFWXX AND JCZBJGDL &lt;= CKZFWSX))</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>某医院在某时间段内有多少科室涉及医疗费总额超过某金额</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医院（医疗机构代码）在（时间段）内有多少科室涉及医疗费总额超过（大实数）元</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医保表</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医院</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>复杂</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>某医院在某时间段内有多少科室涉及医疗费总额不低于某金额</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>某医院在某时间段内有多少科室涉及医疗费总额低于某金额</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>某医院在某时间段内有多少科室涉及医疗费总额不超过某金额</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医院（医疗机构代码）在（时间段）内有多少科室涉及医疗费总额不低于（大实数）元</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医院（医疗机构代码）在（时间段）内有多少科室涉及医疗费总额低于（大实数）元</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医院（医疗机构代码）在（时间段）内有多少科室涉及医疗费总额不超过（大实数）元</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>某医院有多少科室的平均医疗住院时长超过一定天数</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医院（医疗机构代码）有多少科室的平均医疗住院时长超过（整数）天</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医保</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>简单</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>某医院有多少科室的最长医疗住院时长少于一定天数</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>某医院有多少科室的最短医疗住院时长超过一定天数</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医院（医疗机构代码）有多少科室的最长医疗住院时长少于（整数）天</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医院（医疗机构代码）有多少科室的最短医疗住院时长超过（整数）天</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>某医院在某时间段内有多少科室在门诊就诊中开出超过一定数量的检验报告单</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医院（医疗机构代码）在（时间段）内有多少科室在门诊就诊中开出超过（整数）张检验报告单</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医院</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>某医院在某时间段内有多少科室在门诊就诊中开出不少于一定数量的检验报告单</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>某医院在某时间段内有多少科室在门诊就诊中开出少于一定数量的检验报告单</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>某医院在某时间段内有多少科室在门诊就诊中开出不超过一定数量的检验报告单</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医院（医疗机构代码）在（时间段）内有多少科室在门诊就诊中开出不少于（整数）张检验报告单</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医院（医疗机构代码）在（时间段）内有多少科室在门诊就诊中开出少于（整数）张检验报告单</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>医院（医疗机构代码）在（时间段）内有多少科室在门诊就诊中开出不超过（整数）张检验报告单</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT t_kc21.MED_ORG_DEPT_CD FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &gt; $4) as T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT t_kc21.MED_ORG_DEPT_CD FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &gt;= $4) as T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT t_kc21.MED_ORG_DEPT_CD FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &lt; $4) as T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT t_kc21.MED_ORG_DEPT_CD FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD HAVING SUM(t_kc24.MED_AMOUT) &lt;= $4) as T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT MED_ORG_DEPT_CD FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD HAVING AVG(IN_HOSP_DAYS) &gt; $2) as T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT MED_ORG_DEPT_CD FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD HAVING MAX(IN_HOSP_DAYS) &lt; $2) as T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT MED_ORG_DEPT_CD FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD HAVING MIN(IN_HOSP_DAYS) &gt; $2) as T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT jybgb.KSBM FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &gt; $4) as T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT jybgb.KSBM FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &gt;= $4) as T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT jybgb.KSBM FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &lt; $4) as T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) FROM (SELECT jybgb.KSBM FROM mzjzjlb JOIN jybgb ON mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE mzjzjlb.YLJGDM = $1 AND jybgb.BGRQ BETWEEN $2 AND $3 GROUP BY jybgb.KSBM HAVING COUNT(*) &lt;= $4) as T</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4182,11 +4158,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB414"/>
+  <dimension ref="A1:AB412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C387" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C414" sqref="C414"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5094,7 +5068,7 @@
         <v>51</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>1083</v>
+        <v>1077</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>19</v>
@@ -15390,7 +15364,7 @@
         <v>672</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>1089</v>
+        <v>1083</v>
       </c>
       <c r="D258" s="4" t="s">
         <v>19</v>
@@ -15522,7 +15496,7 @@
         <v>678</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>1090</v>
+        <v>1084</v>
       </c>
       <c r="D261" s="4" t="s">
         <v>19</v>
@@ -15566,7 +15540,7 @@
         <v>679</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>1091</v>
+        <v>1085</v>
       </c>
       <c r="D262" s="4" t="s">
         <v>19</v>
@@ -15610,7 +15584,7 @@
         <v>681</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>1088</v>
+        <v>1082</v>
       </c>
       <c r="D263" s="4" t="s">
         <v>19</v>
@@ -19194,7 +19168,7 @@
         <v>944</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="D354" s="5" t="s">
         <v>945</v>
@@ -19217,7 +19191,7 @@
         <v>947</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="D355" s="5" t="s">
         <v>945</v>
@@ -19237,280 +19211,280 @@
         <v>948</v>
       </c>
       <c r="B356" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="C356" s="1" t="s">
         <v>950</v>
-      </c>
-      <c r="C356" s="1" t="s">
-        <v>965</v>
       </c>
       <c r="D356" s="5" t="s">
         <v>945</v>
       </c>
       <c r="E356" s="5" t="s">
-        <v>946</v>
+        <v>951</v>
       </c>
       <c r="F356" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G356" s="5" t="s">
-        <v>887</v>
+        <v>952</v>
       </c>
     </row>
     <row r="357" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>966</v>
+        <v>956</v>
       </c>
       <c r="D357" s="5" t="s">
         <v>945</v>
       </c>
       <c r="E357" s="5" t="s">
-        <v>946</v>
+        <v>951</v>
       </c>
       <c r="F357" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G357" s="5" t="s">
-        <v>887</v>
+        <v>952</v>
       </c>
     </row>
     <row r="358" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>954</v>
+        <v>957</v>
       </c>
       <c r="D358" s="5" t="s">
         <v>945</v>
       </c>
       <c r="E358" s="5" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
       <c r="F358" s="5">
         <v>5</v>
       </c>
       <c r="G358" s="5" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
     </row>
     <row r="359" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="D359" s="5" t="s">
         <v>945</v>
       </c>
       <c r="E359" s="5" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
       <c r="F359" s="5">
         <v>5</v>
       </c>
       <c r="G359" s="5" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
     </row>
     <row r="360" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
-        <v>952</v>
+        <v>961</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>958</v>
+        <v>962</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D360" s="5" t="s">
-        <v>945</v>
+        <v>964</v>
       </c>
       <c r="E360" s="5" t="s">
-        <v>955</v>
+        <v>965</v>
       </c>
       <c r="F360" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G360" s="5" t="s">
-        <v>956</v>
+        <v>966</v>
       </c>
     </row>
     <row r="361" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
-        <v>952</v>
+        <v>961</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>959</v>
+        <v>967</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>962</v>
+        <v>968</v>
       </c>
       <c r="D361" s="5" t="s">
-        <v>945</v>
+        <v>964</v>
       </c>
       <c r="E361" s="5" t="s">
-        <v>955</v>
+        <v>965</v>
       </c>
       <c r="F361" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G361" s="5" t="s">
-        <v>956</v>
+        <v>966</v>
       </c>
     </row>
     <row r="362" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>967</v>
+        <v>974</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>968</v>
+        <v>975</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>969</v>
+        <v>977</v>
       </c>
       <c r="D362" s="5" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="E362" s="5" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="F362" s="5">
         <v>8</v>
       </c>
       <c r="G362" s="5" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
     </row>
     <row r="363" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
-        <v>967</v>
+        <v>974</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>973</v>
+        <v>976</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>974</v>
+        <v>978</v>
       </c>
       <c r="D363" s="5" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="E363" s="5" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="F363" s="5">
         <v>8</v>
       </c>
       <c r="G363" s="5" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
     </row>
     <row r="364" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
-        <v>980</v>
+        <v>969</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>981</v>
+        <v>970</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>983</v>
+        <v>972</v>
       </c>
       <c r="D364" s="5" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="E364" s="5" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="F364" s="5">
         <v>8</v>
       </c>
       <c r="G364" s="5" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
     </row>
     <row r="365" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
-        <v>980</v>
+        <v>969</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>982</v>
+        <v>971</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>984</v>
+        <v>973</v>
       </c>
       <c r="D365" s="5" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="E365" s="5" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="F365" s="5">
         <v>8</v>
       </c>
       <c r="G365" s="5" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
     </row>
     <row r="366" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
-        <v>975</v>
+        <v>979</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>976</v>
+        <v>980</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>978</v>
+        <v>982</v>
       </c>
       <c r="D366" s="5" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="E366" s="5" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="F366" s="5">
         <v>8</v>
       </c>
       <c r="G366" s="5" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
     </row>
     <row r="367" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
-        <v>975</v>
+        <v>979</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>977</v>
+        <v>981</v>
       </c>
       <c r="C367" s="1" t="s">
-        <v>979</v>
+        <v>983</v>
       </c>
       <c r="D367" s="5" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="E367" s="5" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="F367" s="5">
         <v>8</v>
       </c>
       <c r="G367" s="5" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
     </row>
     <row r="368" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B368" s="1" t="s">
         <v>986</v>
@@ -19519,16 +19493,16 @@
         <v>988</v>
       </c>
       <c r="D368" s="5" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="E368" s="5" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="F368" s="5">
         <v>8</v>
       </c>
       <c r="G368" s="5" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
     </row>
     <row r="369" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -19542,16 +19516,16 @@
         <v>989</v>
       </c>
       <c r="D369" s="5" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="E369" s="5" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="F369" s="5">
         <v>8</v>
       </c>
       <c r="G369" s="5" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
     </row>
     <row r="370" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -19565,16 +19539,16 @@
         <v>994</v>
       </c>
       <c r="D370" s="5" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="E370" s="5" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="F370" s="5">
         <v>8</v>
       </c>
       <c r="G370" s="5" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
     </row>
     <row r="371" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -19588,16 +19562,16 @@
         <v>995</v>
       </c>
       <c r="D371" s="5" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="E371" s="5" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="F371" s="5">
         <v>8</v>
       </c>
       <c r="G371" s="5" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
     </row>
     <row r="372" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -19605,257 +19579,257 @@
         <v>996</v>
       </c>
       <c r="B372" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="C372" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="C372" s="1" t="s">
+      <c r="D372" s="5" t="s">
+        <v>999</v>
+      </c>
+      <c r="E372" s="5" t="s">
         <v>1000</v>
-      </c>
-      <c r="D372" s="5" t="s">
-        <v>970</v>
-      </c>
-      <c r="E372" s="5" t="s">
-        <v>971</v>
       </c>
       <c r="F372" s="5">
         <v>8</v>
       </c>
       <c r="G372" s="5" t="s">
-        <v>972</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="373" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B373" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D373" s="5" t="s">
         <v>999</v>
       </c>
-      <c r="C373" s="1" t="s">
-        <v>1001</v>
-      </c>
-      <c r="D373" s="5" t="s">
-        <v>970</v>
-      </c>
       <c r="E373" s="5" t="s">
-        <v>971</v>
+        <v>1000</v>
       </c>
       <c r="F373" s="5">
         <v>8</v>
       </c>
       <c r="G373" s="5" t="s">
-        <v>972</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="374" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="C374" s="1" t="s">
-        <v>1004</v>
+        <v>1007</v>
       </c>
       <c r="D374" s="5" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="E374" s="5" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="F374" s="5">
         <v>8</v>
       </c>
       <c r="G374" s="5" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="375" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="B375" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C375" s="1" t="s">
         <v>1008</v>
       </c>
-      <c r="C375" s="1" t="s">
-        <v>1009</v>
-      </c>
       <c r="D375" s="5" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="E375" s="5" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="F375" s="5">
         <v>8</v>
       </c>
       <c r="G375" s="5" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="376" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>1010</v>
+        <v>1023</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>1011</v>
+        <v>1027</v>
       </c>
       <c r="C376" s="1" t="s">
-        <v>1013</v>
+        <v>1031</v>
       </c>
       <c r="D376" s="5" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="E376" s="5" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="F376" s="5">
         <v>8</v>
       </c>
       <c r="G376" s="5" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="377" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
-        <v>1010</v>
+        <v>1024</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>1012</v>
+        <v>1028</v>
       </c>
       <c r="C377" s="1" t="s">
-        <v>1014</v>
+        <v>1032</v>
       </c>
       <c r="D377" s="5" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="E377" s="5" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="F377" s="5">
         <v>8</v>
       </c>
       <c r="G377" s="5" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="378" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B378" s="1" t="s">
         <v>1029</v>
       </c>
-      <c r="B378" s="1" t="s">
+      <c r="C378" s="1" t="s">
         <v>1033</v>
       </c>
-      <c r="C378" s="1" t="s">
-        <v>1037</v>
-      </c>
       <c r="D378" s="5" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="E378" s="5" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="F378" s="5">
         <v>8</v>
       </c>
       <c r="G378" s="5" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="379" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B379" s="1" t="s">
         <v>1030</v>
       </c>
-      <c r="B379" s="1" t="s">
+      <c r="C379" s="1" t="s">
         <v>1034</v>
       </c>
-      <c r="C379" s="1" t="s">
-        <v>1038</v>
-      </c>
       <c r="D379" s="5" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="E379" s="5" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="F379" s="5">
         <v>8</v>
       </c>
       <c r="G379" s="5" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="380" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
-        <v>1031</v>
+        <v>1009</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>1035</v>
+        <v>1010</v>
       </c>
       <c r="C380" s="1" t="s">
-        <v>1039</v>
+        <v>1011</v>
       </c>
       <c r="D380" s="5" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="E380" s="5" t="s">
-        <v>1006</v>
+        <v>1012</v>
       </c>
       <c r="F380" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G380" s="5" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="381" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
-        <v>1032</v>
+        <v>1014</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>1036</v>
+        <v>1015</v>
       </c>
       <c r="C381" s="1" t="s">
-        <v>1040</v>
+        <v>1016</v>
       </c>
       <c r="D381" s="5" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="E381" s="5" t="s">
-        <v>1006</v>
+        <v>1012</v>
       </c>
       <c r="F381" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G381" s="5" t="s">
-        <v>1007</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="382" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>1016</v>
+        <v>1020</v>
       </c>
       <c r="C382" s="1" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="D382" s="5" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="E382" s="5" t="s">
-        <v>1018</v>
+        <v>1012</v>
       </c>
       <c r="F382" s="5">
         <v>6</v>
       </c>
       <c r="G382" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="383" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="B383" s="1" t="s">
         <v>1021</v>
@@ -19864,154 +19838,154 @@
         <v>1022</v>
       </c>
       <c r="D383" s="5" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="E383" s="5" t="s">
-        <v>1018</v>
+        <v>1012</v>
       </c>
       <c r="F383" s="5">
         <v>6</v>
       </c>
       <c r="G383" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="384" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
-        <v>1023</v>
+        <v>1035</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>1026</v>
+        <v>1036</v>
       </c>
       <c r="C384" s="1" t="s">
-        <v>1025</v>
+        <v>1037</v>
       </c>
       <c r="D384" s="5" t="s">
-        <v>1005</v>
+        <v>1038</v>
       </c>
       <c r="E384" s="5" t="s">
-        <v>1018</v>
+        <v>1039</v>
       </c>
       <c r="F384" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G384" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="385" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
-        <v>1024</v>
+        <v>1035</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>1027</v>
+        <v>1040</v>
       </c>
       <c r="C385" s="1" t="s">
-        <v>1028</v>
+        <v>1041</v>
       </c>
       <c r="D385" s="5" t="s">
-        <v>1005</v>
+        <v>1038</v>
       </c>
       <c r="E385" s="5" t="s">
-        <v>1018</v>
+        <v>1039</v>
       </c>
       <c r="F385" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G385" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="386" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="C386" s="1" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="D386" s="5" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="E386" s="5" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="F386" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G386" s="5" t="s">
-        <v>1019</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="387" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B387" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C387" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D387" s="5" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E387" s="5" t="s">
         <v>1046</v>
       </c>
-      <c r="C387" s="1" t="s">
+      <c r="F387" s="5">
+        <v>6</v>
+      </c>
+      <c r="G387" s="5" t="s">
         <v>1047</v>
-      </c>
-      <c r="D387" s="5" t="s">
-        <v>1044</v>
-      </c>
-      <c r="E387" s="5" t="s">
-        <v>1045</v>
-      </c>
-      <c r="F387" s="5">
-        <v>4</v>
-      </c>
-      <c r="G387" s="5" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="388" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>1049</v>
+        <v>1052</v>
       </c>
       <c r="C388" s="1" t="s">
-        <v>1050</v>
+        <v>1054</v>
       </c>
       <c r="D388" s="5" t="s">
-        <v>1051</v>
+        <v>1045</v>
       </c>
       <c r="E388" s="5" t="s">
-        <v>1052</v>
+        <v>1046</v>
       </c>
       <c r="F388" s="5">
         <v>6</v>
       </c>
       <c r="G388" s="5" t="s">
-        <v>1053</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="389" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>1048</v>
+        <v>1051</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="C389" s="1" t="s">
         <v>1055</v>
       </c>
       <c r="D389" s="5" t="s">
-        <v>1051</v>
+        <v>1045</v>
       </c>
       <c r="E389" s="5" t="s">
-        <v>1052</v>
+        <v>1046</v>
       </c>
       <c r="F389" s="5">
         <v>6</v>
       </c>
       <c r="G389" s="5" t="s">
-        <v>1053</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="390" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -20019,45 +19993,45 @@
         <v>1056</v>
       </c>
       <c r="B390" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C390" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D390" s="5" t="s">
         <v>1058</v>
       </c>
-      <c r="C390" s="1" t="s">
-        <v>1060</v>
-      </c>
-      <c r="D390" s="5" t="s">
-        <v>1051</v>
-      </c>
       <c r="E390" s="5" t="s">
-        <v>1052</v>
+        <v>1059</v>
       </c>
       <c r="F390" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G390" s="5" t="s">
-        <v>1053</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="391" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C391" s="1" t="s">
         <v>1061</v>
       </c>
       <c r="D391" s="5" t="s">
-        <v>1051</v>
+        <v>1058</v>
       </c>
       <c r="E391" s="5" t="s">
-        <v>1052</v>
+        <v>1059</v>
       </c>
       <c r="F391" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G391" s="5" t="s">
-        <v>1053</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="392" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -20065,45 +20039,45 @@
         <v>1062</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="C392" s="1" t="s">
-        <v>1087</v>
+        <v>1066</v>
       </c>
       <c r="D392" s="5" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
       <c r="E392" s="5" t="s">
-        <v>1065</v>
+        <v>1059</v>
       </c>
       <c r="F392" s="5">
         <v>5</v>
       </c>
       <c r="G392" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="393" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="C393" s="1" t="s">
         <v>1067</v>
       </c>
       <c r="D393" s="5" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
       <c r="E393" s="5" t="s">
-        <v>1065</v>
+        <v>1059</v>
       </c>
       <c r="F393" s="5">
         <v>5</v>
       </c>
       <c r="G393" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="394" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -20114,479 +20088,433 @@
         <v>1070</v>
       </c>
       <c r="C394" s="1" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="D394" s="5" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
       <c r="E394" s="5" t="s">
-        <v>1065</v>
+        <v>1059</v>
       </c>
       <c r="F394" s="5">
         <v>5</v>
       </c>
       <c r="G394" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="395" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B395" s="1" t="s">
         <v>1071</v>
       </c>
       <c r="C395" s="1" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="D395" s="5" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
       <c r="E395" s="5" t="s">
-        <v>1065</v>
+        <v>1059</v>
       </c>
       <c r="F395" s="5">
         <v>5</v>
       </c>
       <c r="G395" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="396" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
-        <v>1074</v>
+        <v>1069</v>
       </c>
       <c r="B396" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C396" s="1" t="s">
         <v>1076</v>
       </c>
-      <c r="C396" s="1" t="s">
-        <v>1080</v>
-      </c>
       <c r="D396" s="5" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
       <c r="E396" s="5" t="s">
-        <v>1065</v>
+        <v>1059</v>
       </c>
       <c r="F396" s="5">
         <v>5</v>
       </c>
       <c r="G396" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="397" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
-        <v>1074</v>
+        <v>1069</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
       <c r="C397" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="D397" s="5" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
       <c r="E397" s="5" t="s">
-        <v>1065</v>
+        <v>1059</v>
       </c>
       <c r="F397" s="5">
         <v>5</v>
       </c>
       <c r="G397" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="398" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
-        <v>1075</v>
+        <v>1078</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="C398" s="1" t="s">
-        <v>1082</v>
+        <v>1135</v>
       </c>
       <c r="D398" s="5" t="s">
-        <v>1064</v>
+        <v>1086</v>
       </c>
       <c r="E398" s="5" t="s">
-        <v>1065</v>
+        <v>1087</v>
       </c>
       <c r="F398" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G398" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="399" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
-        <v>1075</v>
+        <v>1078</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>1079</v>
+        <v>1088</v>
       </c>
       <c r="C399" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D399" s="5" t="s">
         <v>1086</v>
       </c>
-      <c r="D399" s="5" t="s">
-        <v>1064</v>
-      </c>
       <c r="E399" s="5" t="s">
-        <v>1065</v>
+        <v>1087</v>
       </c>
       <c r="F399" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G399" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="400" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
-        <v>1084</v>
+        <v>1090</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>1085</v>
+        <v>1092</v>
       </c>
       <c r="C400" s="1" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="D400" s="5" t="s">
-        <v>1092</v>
+        <v>1086</v>
       </c>
       <c r="E400" s="5" t="s">
-        <v>1094</v>
+        <v>1087</v>
       </c>
       <c r="F400" s="5">
         <v>2</v>
       </c>
       <c r="G400" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="401" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
-        <v>1084</v>
+        <v>1091</v>
       </c>
       <c r="B401" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C401" s="1" t="s">
         <v>1095</v>
       </c>
-      <c r="C401" s="1" t="s">
-        <v>1096</v>
-      </c>
       <c r="D401" s="5" t="s">
-        <v>1092</v>
+        <v>1086</v>
       </c>
       <c r="E401" s="5" t="s">
-        <v>1094</v>
+        <v>1087</v>
       </c>
       <c r="F401" s="5">
         <v>2</v>
       </c>
       <c r="G401" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="402" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B402" s="1" t="s">
         <v>1097</v>
       </c>
-      <c r="B402" s="1" t="s">
+      <c r="C402" s="1" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D402" s="5" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E402" s="5" t="s">
         <v>1099</v>
       </c>
-      <c r="C402" s="1" t="s">
-        <v>1101</v>
-      </c>
-      <c r="D402" s="5" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E402" s="5" t="s">
-        <v>1094</v>
-      </c>
       <c r="F402" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G402" s="5" t="s">
-        <v>1019</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="403" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B403" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C403" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D403" s="5" t="s">
         <v>1098</v>
       </c>
-      <c r="B403" s="1" t="s">
+      <c r="E403" s="5" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F403" s="5">
+        <v>4</v>
+      </c>
+      <c r="G403" s="5" t="s">
         <v>1100</v>
-      </c>
-      <c r="C403" s="1" t="s">
-        <v>1102</v>
-      </c>
-      <c r="D403" s="5" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E403" s="5" t="s">
-        <v>1094</v>
-      </c>
-      <c r="F403" s="5">
-        <v>2</v>
-      </c>
-      <c r="G403" s="5" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="404" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="C404" s="1" t="s">
-        <v>1131</v>
+        <v>1126</v>
       </c>
       <c r="D404" s="5" t="s">
-        <v>1105</v>
+        <v>1098</v>
       </c>
       <c r="E404" s="5" t="s">
-        <v>1106</v>
+        <v>1099</v>
       </c>
       <c r="F404" s="5">
         <v>4</v>
       </c>
       <c r="G404" s="5" t="s">
-        <v>1107</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="405" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
-        <v>1108</v>
+        <v>1103</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>1111</v>
+        <v>1106</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>1132</v>
+        <v>1127</v>
       </c>
       <c r="D405" s="5" t="s">
-        <v>1105</v>
+        <v>1098</v>
       </c>
       <c r="E405" s="5" t="s">
-        <v>1106</v>
+        <v>1099</v>
       </c>
       <c r="F405" s="5">
         <v>4</v>
       </c>
       <c r="G405" s="5" t="s">
-        <v>1107</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="406" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C406" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D406" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E406" s="5" t="s">
         <v>1109</v>
       </c>
-      <c r="B406" s="1" t="s">
-        <v>1112</v>
-      </c>
-      <c r="C406" s="1" t="s">
-        <v>1133</v>
-      </c>
-      <c r="D406" s="5" t="s">
-        <v>1105</v>
-      </c>
-      <c r="E406" s="5" t="s">
-        <v>1106</v>
-      </c>
       <c r="F406" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G406" s="5" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="407" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="B407" s="1" t="s">
         <v>1113</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>1134</v>
+        <v>1129</v>
       </c>
       <c r="D407" s="5" t="s">
-        <v>1105</v>
+        <v>1038</v>
       </c>
       <c r="E407" s="5" t="s">
-        <v>1106</v>
+        <v>1109</v>
       </c>
       <c r="F407" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G407" s="5" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="408" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B408" s="1" t="s">
         <v>1114</v>
       </c>
-      <c r="B408" s="1" t="s">
-        <v>1115</v>
-      </c>
       <c r="C408" s="1" t="s">
-        <v>1135</v>
+        <v>1130</v>
       </c>
       <c r="D408" s="5" t="s">
-        <v>1044</v>
+        <v>1038</v>
       </c>
       <c r="E408" s="5" t="s">
-        <v>1116</v>
+        <v>1109</v>
       </c>
       <c r="F408" s="5">
         <v>6</v>
       </c>
       <c r="G408" s="5" t="s">
-        <v>1117</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="409" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>1136</v>
+        <v>1131</v>
       </c>
       <c r="D409" s="5" t="s">
-        <v>1044</v>
+        <v>1058</v>
       </c>
       <c r="E409" s="5" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="F409" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G409" s="5" t="s">
-        <v>1117</v>
+        <v>966</v>
       </c>
     </row>
     <row r="410" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B410" s="1" t="s">
         <v>1121</v>
       </c>
       <c r="C410" s="1" t="s">
-        <v>1137</v>
+        <v>1132</v>
       </c>
       <c r="D410" s="5" t="s">
-        <v>1044</v>
+        <v>1058</v>
       </c>
       <c r="E410" s="5" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="F410" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G410" s="5" t="s">
-        <v>1117</v>
+        <v>966</v>
       </c>
     </row>
     <row r="411" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B411" s="1" t="s">
         <v>1122</v>
       </c>
-      <c r="B411" s="1" t="s">
-        <v>1123</v>
-      </c>
       <c r="C411" s="1" t="s">
-        <v>1138</v>
+        <v>1133</v>
       </c>
       <c r="D411" s="5" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
       <c r="E411" s="5" t="s">
-        <v>1124</v>
+        <v>1117</v>
       </c>
       <c r="F411" s="5">
         <v>4</v>
       </c>
       <c r="G411" s="5" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
     </row>
     <row r="412" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
-        <v>1125</v>
+        <v>1120</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>1128</v>
+        <v>1123</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>1139</v>
+        <v>1134</v>
       </c>
       <c r="D412" s="5" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
       <c r="E412" s="5" t="s">
-        <v>1124</v>
+        <v>1117</v>
       </c>
       <c r="F412" s="5">
         <v>4</v>
       </c>
       <c r="G412" s="5" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="413" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A413" s="1" t="s">
-        <v>1126</v>
-      </c>
-      <c r="B413" s="1" t="s">
-        <v>1129</v>
-      </c>
-      <c r="C413" s="1" t="s">
-        <v>1140</v>
-      </c>
-      <c r="D413" s="5" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E413" s="5" t="s">
-        <v>1124</v>
-      </c>
-      <c r="F413" s="5">
-        <v>4</v>
-      </c>
-      <c r="G413" s="5" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="414" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A414" s="1" t="s">
-        <v>1127</v>
-      </c>
-      <c r="B414" s="1" t="s">
-        <v>1130</v>
-      </c>
-      <c r="C414" s="1" t="s">
-        <v>1141</v>
-      </c>
-      <c r="D414" s="5" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E414" s="5" t="s">
-        <v>1124</v>
-      </c>
-      <c r="F414" s="5">
-        <v>4</v>
-      </c>
-      <c r="G414" s="5" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: new templates for intersect
</commit_message>
<xml_diff>
--- a/dataset/templates.xlsx
+++ b/dataset/templates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2422" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2482" uniqueCount="1175">
   <si>
     <t>一家医院调取患者之前在其他所有医院的就诊、检查数据，医保对可疑的就诊调取医院的就诊信息，与医保数据进行比对</t>
   </si>
@@ -3766,6 +3766,162 @@
   </si>
   <si>
     <t>(SELECT jybgb.BGDH FROM hz_info JOIN mzjzjlb JOIN jybgb ON hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX AND mzjzjlb.YLJGDM = jybgb.YLJGDM AND mzjzjlb.JZLSH = jybgb.JZLSH WHERE hz_info.RYBH = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &lt; CKZFWXX OR JCZBJGDL &gt; CKZFWSX)) UNION (SELECT jybgb.BGDH FROM hz_info JOIN zyjzjlb JOIN jybgb ON hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX AND zyjzjlb.YLJGDM = jybgb.YLJGDM AND zyjzjlb.JZLSH = jybgb.JZLSH WHERE hz_info.RYBH = $1 AND jybgb.BGDH NOT IN (SELECT BGDH FROM jyjgzbb WHERE JCZBJGDL &lt; CKZFWXX OR JCZBJGDL &gt; CKZFWSX))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某次医疗就诊中患者被开出的所有药品编码和名称及其金额，去除金额最低的一项，其余按金额降序排列</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医疗就诊（医疗就诊ID）中患者被开出的所有药品编码和名称及其金额，去除金额最低的药品，其余按金额降序排列</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗就诊（医疗就诊ID）与医疗就诊（医疗就诊ID）中开出了哪些名称相同的药品？列出这些药品的名称</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>两次医疗就诊中开出了哪些名称相同的药品？列出这些药品的名称</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(SELECT SOC_SRT_DIRE_NM FROM t_kc22 WHERE MED_CLINIC_ID = $1) INTERSECT (SELECT SOC_SRT_DIRE_NM FROM t_kc22 WHERE MED_CLINIC_ID = $2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>两份检验报告单中是否有名称相同的检测指标？列出这些检测指标名称</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>检验报告单（检验报告单号）与检验报告单（检验报告单号）中是否有名称相同的检测指标？列出这些检测指标名称</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(SELECT JCZBMC FROM jyjgzbb WHERE BGDH = $1) INTERSECT (SELECT JCZBMC FROM jyjgzbb WHERE BGDH = $2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医生</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>两次医疗就诊中开出了哪些名称相同的药品？列出这些药品的名称和金额以及对应的医疗就诊ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗就诊（医疗就诊ID）与医疗就诊（医疗就诊ID）中开出了哪些名称相同的药品？列出这些药品的名称和金额以及对应的医疗就诊ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT SOC_SRT_DIRE_NM, AMOUNT, MED_CLINIC_ID FROM t_kc22 WHERE (MED_CLINIC_ID = $1 OR MED_CLINIC_ID = $2) AND SOC_SRT_DIRE_NM IN ((SELECT SOC_SRT_DIRE_NM FROM t_kc22 WHERE MED_CLINIC_ID = $1) INTERSECT (SELECT SOC_SRT_DIRE_NM FROM t_kc22 WHERE MED_CLINIC_ID = $2))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(SELECT SOC_SRT_DIRE_NM, AMOUNT, MED_CLINIC_ID FROM t_kc22 WHERE MED_CLINIC_ID = $1 AND SOC_SRT_DIRE_NM IN (SELECT SOC_SRT_DIRE_NM FROM t_kc22 WHERE MED_CLINIC_ID = $2)) UNION (SELECT SOC_SRT_DIRE_NM, AMOUNT, MED_CLINIC_ID FROM t_kc22 WHERE MED_CLINIC_ID = $2 AND SOC_SRT_DIRE_NM IN (SELECT SOC_SRT_DIRE_NM FROM t_kc22 WHERE MED_CLINIC_ID = $1))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>两份检验报告单中是否有名称相同的检测指标？列出这些检测指标名称、检测指标结果定量及其单位、对应的检验报告单号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>检验报告单（检验报告单号）与检验报告单（检验报告单号）中是否有名称相同的检测指标？列出这些检测指标名称、检测指标结果定量及其单位、对应的检验报告单号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT JCZBMC, JCZBJGDL, JCZBJGDW, BGDH FROM jyjgzbb WHERE (BGDH = $1 OR BGDH = $2) AND JCZBMC IN ((SELECT JCZBMC FROM jyjgzbb WHERE BGDH = $1) INTERSECT (SELECT JCZBMC FROM jyjgzbb WHERE BGDH = $2))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(SELECT JCZBMC, JCZBJGDL, JCZBJGDW, BGDH FROM jyjgzbb WHERE BGDH = $1 AND JCZBMC IN (SELECT JCZBMC FROM jyjgzbb WHERE BGDH = $2)) UNION (SELECT JCZBMC, JCZBJGDL, JCZBJGDW, BGDH FROM jyjgzbb WHERE BGDH = $2 AND JCZBMC IN (SELECT JCZBMC FROM jyjgzbb WHERE BGDH = $1))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某次医疗就诊中有哪些人申请超过若干份检验报告单？列出这些申请人工号和姓名</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗就诊（门诊就诊流水号或住院就诊流水号）中有哪些人申请超过（整数）份检验报告单？列出这些申请人工号和姓名</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT SQRGH, SQRXM FROM jybgb WHERE JZLSH = $1 GROUP BY SQRGH HAVING COUNT(*) &gt; $2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某次医疗就诊中有哪些人报告超过若干份检验报告单？列出这些报告人工号和姓名</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某次医疗就诊中有哪些人审核超过若干份检验报告单？列出这些审核人工号和姓名</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗就诊（门诊就诊流水号或住院就诊流水号）中有哪些人报告超过（整数）份检验报告单？列出这些报告人工号和姓名</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗就诊（门诊就诊流水号或住院就诊流水号）中有哪些人审核超过（整数）份检验报告单？列出这些审核人工号和姓名</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT BGRGH, BGRXM FROM jybgb WHERE JZLSH = $1 GROUP BY BGRGH HAVING COUNT(*) &gt; $2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT SHRGH, SHRXM FROM jybgb WHERE JZLSH = $1 GROUP BY SHRGH HAVING COUNT(*) &gt; $2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM, AMOUNT FROM t_kc22 WHERE MED_CLINIC_ID = $1 AND AMOUNT &gt; (SELECT MIN(AMOUNT) FROM t_kc22 WHERE MED_CLINIC_ID = $1) ORDER BY AMOUNT DESC</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4158,14 +4314,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB412"/>
+  <dimension ref="A1:AB422"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="101" customWidth="1"/>
-    <col min="2" max="2" width="110.6640625" customWidth="1"/>
+    <col min="1" max="1" width="102.88671875" customWidth="1"/>
+    <col min="2" max="2" width="140.77734375" customWidth="1"/>
     <col min="3" max="3" width="255.77734375" customWidth="1"/>
     <col min="4" max="28" width="14" customWidth="1"/>
   </cols>
@@ -20517,6 +20673,236 @@
         <v>966</v>
       </c>
     </row>
+    <row r="413" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A413" s="1" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B413" s="1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C413" s="1" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D413" s="5" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E413" s="5" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F413" s="5">
+        <v>8</v>
+      </c>
+      <c r="G413" s="5" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="414" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A414" s="1" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B414" s="1" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C414" s="1" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D414" s="5" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E414" s="5" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F414" s="5">
+        <v>8</v>
+      </c>
+      <c r="G414" s="5" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="415" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A415" s="1" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B415" s="1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D415" s="5" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E415" s="5" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F415" s="5">
+        <v>8</v>
+      </c>
+      <c r="G415" s="5" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="416" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A416" s="1" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B416" s="1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C416" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D416" s="5" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E416" s="5" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F416" s="5">
+        <v>8</v>
+      </c>
+      <c r="G416" s="5" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="417" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A417" s="1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B417" s="1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C417" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D417" s="5" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E417" s="5" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F417" s="5">
+        <v>2</v>
+      </c>
+      <c r="G417" s="5" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="418" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A418" s="1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B418" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C418" s="1" t="s">
+        <v>1160</v>
+      </c>
+      <c r="D418" s="5" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E418" s="5" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F418" s="5">
+        <v>2</v>
+      </c>
+      <c r="G418" s="5" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="419" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A419" s="1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B419" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C419" s="1" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D419" s="5" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E419" s="5" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F419" s="5">
+        <v>2</v>
+      </c>
+      <c r="G419" s="5" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="420" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A420" s="1" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B420" s="1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C420" s="1" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D420" s="5" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E420" s="5" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F420" s="5">
+        <v>4</v>
+      </c>
+      <c r="G420" s="5" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="421" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A421" s="1" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B421" s="1" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C421" s="1" t="s">
+        <v>1172</v>
+      </c>
+      <c r="D421" s="5" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E421" s="5" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F421" s="5">
+        <v>4</v>
+      </c>
+      <c r="G421" s="5" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="422" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A422" s="1" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B422" s="1" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C422" s="1" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D422" s="5" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E422" s="5" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F422" s="5">
+        <v>4</v>
+      </c>
+      <c r="G422" s="5" t="s">
+        <v>1167</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: statistics for grammar rules
</commit_message>
<xml_diff>
--- a/dataset/templates.xlsx
+++ b/dataset/templates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2482" uniqueCount="1175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2560" uniqueCount="1227">
   <si>
     <t>一家医院调取患者之前在其他所有医院的就诊、检查数据，医保对可疑的就诊调取医院的就诊信息，与医保数据进行比对</t>
   </si>
@@ -3922,6 +3922,214 @@
   </si>
   <si>
     <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM, AMOUNT FROM t_kc22 WHERE MED_CLINIC_ID = $1 AND AMOUNT &gt; (SELECT MIN(AMOUNT) FROM t_kc22 WHERE MED_CLINIC_ID = $1) ORDER BY AMOUNT DESC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某医院各科室的编码和名称以及平均住院时长，并按平均住院时长升序排序</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医院（医疗机构代码）各科室的编码和名称以及平均住院时长，并按平均住院时长升序排序</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_ORG_DEPT_CD, MED_ORG_DEPT_NM, AVG(IN_HOSP_DAYS) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD ORDER BY AVG(IN_HOSP_DAYS) ASC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医疗费总额与某次医疗就诊相同的医疗就诊记录的ID、人员ID、人员姓名、公民身份号码、人员性别、人员年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医疗费总额与医疗就诊（医疗就诊ID）相同的医疗就诊记录的ID、人员ID、人员姓名、公民身份号码、人员性别、人员年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT t_kc21.MED_CLINIC_ID, t_kc21.PERSON_ID, t_kc21.PERSON_NM, t_kc21.IDENTITY_CARD, t_kc21.PERSON_SEX, t_kc21.PERSON_AGE FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc24.MED_AMOUT = (SELECT MED_AMOUT FROM t_kc24 WHERE MED_CLINIC_ID = $1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某张检验报告单的所有检验指标的代码、名称、结果定性、结果定量、结果定量单位、参考值范围下限与上限</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出检验报告单（检验报告单号）的所有检验指标的代码、名称、结果定性、结果定量、结果定量单位、参考值范围下限与上限</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT JCZBDM, JCZBMC, JCZBJGDX, JCZBJGDL, JCZBJGDW, CKZFWXX, CKZFWSX FROM jyjgzbb WHERE BGDH = $1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医生</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>找出检测指标名称与检测指标结果定量单位和某项检验指标记录相同，且检测指标结果定量小于其的检验指标记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>找出检测指标名称与检测指标结果定量单位和检验指标记录（检验指标流水号）相同，且检测指标结果定量小于其的检验指标记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM jyjgzbb WHERE JCZBMC = (SELECT JCZBMC FROM jyjgzbb WHERE JYZBLSH = $1) AND JCZBJGDW = (SELECT JCZBJGDW FROM jyjgzbb WHERE JYZBLSH = $1) AND JCZBJGDL &lt; (SELECT JCZBJGDL FROM jyjgzbb WHERE JYZBLSH = $1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>找出检测指标名称与检测指标结果定量单位和某项检验指标记录相同，且检测指标结果定量小于等于其的检验指标记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>找出检测指标名称与检测指标结果定量单位和某项检验指标记录相同，且检测指标结果定量大于其的检验指标记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>找出检测指标名称与检测指标结果定量单位和某项检验指标记录相同，且检测指标结果定量大于等于其的检验指标记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>找出检测指标名称、检测指标结果定量单位、检测指标结果定量和某项检验指标记录相同的检验指标记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>找出检测指标名称与检测指标结果定量单位和某项检验指标记录相同，且检测指标结果定量不等于其的检验指标记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>找出检测指标名称与检测指标结果定量单位和检验指标记录（检验指标流水号）相同，且检测指标结果定量小于等于其的检验指标记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>找出检测指标名称与检测指标结果定量单位和检验指标记录（检验指标流水号）相同，且检测指标结果定量大于其的检验指标记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>找出检测指标名称与检测指标结果定量单位和检验指标记录（检验指标流水号）相同，且检测指标结果定量大于等于其的检验指标记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>找出检测指标名称与检测指标结果定量单位和检验指标记录（检验指标流水号）相同，且检测指标结果定量不等于其的检验指标记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>找出检测指标名称、检测指标结果定量单位、检测指标结果定量和检验指标记录（检验指标流水号）相同的检验指标记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM jyjgzbb WHERE JCZBMC = (SELECT JCZBMC FROM jyjgzbb WHERE JYZBLSH = $1) AND JCZBJGDW = (SELECT JCZBJGDW FROM jyjgzbb WHERE JYZBLSH = $1) AND JCZBJGDL &lt;= (SELECT JCZBJGDL FROM jyjgzbb WHERE JYZBLSH = $1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM jyjgzbb WHERE JCZBMC = (SELECT JCZBMC FROM jyjgzbb WHERE JYZBLSH = $1) AND JCZBJGDW = (SELECT JCZBJGDW FROM jyjgzbb WHERE JYZBLSH = $1) AND JCZBJGDL &gt; (SELECT JCZBJGDL FROM jyjgzbb WHERE JYZBLSH = $1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM jyjgzbb WHERE JCZBMC = (SELECT JCZBMC FROM jyjgzbb WHERE JYZBLSH = $1) AND JCZBJGDW = (SELECT JCZBJGDW FROM jyjgzbb WHERE JYZBLSH = $1) AND JCZBJGDL &gt;= (SELECT JCZBJGDL FROM jyjgzbb WHERE JYZBLSH = $1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM jyjgzbb WHERE JCZBMC = (SELECT JCZBMC FROM jyjgzbb WHERE JYZBLSH = $1) AND JCZBJGDW = (SELECT JCZBJGDW FROM jyjgzbb WHERE JYZBLSH = $1) AND JCZBJGDL &lt;&gt; (SELECT JCZBJGDL FROM jyjgzbb WHERE JYZBLSH = $1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM jyjgzbb WHERE JCZBMC = (SELECT JCZBMC FROM jyjgzbb WHERE JYZBLSH = $1) AND JCZBJGDW = (SELECT JCZBJGDW FROM jyjgzbb WHERE JYZBLSH = $1) AND JCZBJGDL = (SELECT JCZBJGDL FROM jyjgzbb WHERE JYZBLSH = $1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据入院诊断疾病编码，列出某医院中不同疾病的平均患者年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据入院诊断疾病编码，列出医院（医疗机构代码）中不同疾病的平均患者年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT IN_DIAG_DIS_CD, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY IN_DIAG_DIS_CD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据入院诊断疾病名称，列出某医院中不同疾病的平均患者年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据出院诊断疾病编码，列出某医院中不同疾病的平均患者年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据出院诊断疾病名称，列出某医院中不同疾病的平均患者年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据入院诊断疾病名称，列出医院（医疗机构代码）中不同疾病的平均患者年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据出院诊断疾病编码，列出医院（医疗机构代码）中不同疾病的平均患者年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据出院诊断疾病名称，列出医院（医疗机构代码）中不同疾病的平均患者年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT IN_DIAG_DIS_NM, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY IN_DIAG_DIS_NM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT OUT_DIAG_DIS_CD, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY OUT_DIAG_DIS_CD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT OUT_DIAG_DIS_NM, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY OUT_DIAG_DIS_NM</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4314,13 +4522,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB422"/>
+  <dimension ref="A1:AB435"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="102.88671875" customWidth="1"/>
+    <col min="1" max="1" width="103.21875" customWidth="1"/>
     <col min="2" max="2" width="140.77734375" customWidth="1"/>
     <col min="3" max="3" width="255.77734375" customWidth="1"/>
     <col min="4" max="28" width="14" customWidth="1"/>
@@ -20903,6 +21111,305 @@
         <v>1167</v>
       </c>
     </row>
+    <row r="423" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A423" s="1" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B423" s="1" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C423" s="1" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D423" s="5" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E423" s="5" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F423" s="5">
+        <v>4</v>
+      </c>
+      <c r="G423" s="5" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="424" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A424" s="1" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B424" s="1" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C424" s="1" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D424" s="5" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E424" s="5" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F424" s="5">
+        <v>6</v>
+      </c>
+      <c r="G424" s="5" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="425" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A425" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B425" s="1" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C425" s="1" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D425" s="5" t="s">
+        <v>1189</v>
+      </c>
+      <c r="E425" s="5" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F425" s="5">
+        <v>2</v>
+      </c>
+      <c r="G425" s="5" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="426" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A426" s="1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B426" s="1" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C426" s="1" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D426" s="5" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E426" s="5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="F426" s="5">
+        <v>6</v>
+      </c>
+      <c r="G426" s="5" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="427" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A427" s="1" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B427" s="1" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C427" s="1" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D427" s="5" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E427" s="5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="F427" s="5">
+        <v>6</v>
+      </c>
+      <c r="G427" s="5" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="428" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A428" s="1" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D428" s="5" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E428" s="5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="F428" s="5">
+        <v>6</v>
+      </c>
+      <c r="G428" s="5" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="429" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A429" s="1" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B429" s="1" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C429" s="1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="D429" s="5" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E429" s="5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="F429" s="5">
+        <v>6</v>
+      </c>
+      <c r="G429" s="5" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="430" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A430" s="1" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B430" s="1" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C430" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D430" s="5" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E430" s="5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="F430" s="5">
+        <v>6</v>
+      </c>
+      <c r="G430" s="5" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="431" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A431" s="1" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B431" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C431" s="1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D431" s="5" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E431" s="5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="F431" s="5">
+        <v>6</v>
+      </c>
+      <c r="G431" s="5" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="432" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A432" s="1" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B432" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C432" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D432" s="5" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E432" s="5" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F432" s="5">
+        <v>6</v>
+      </c>
+      <c r="G432" s="5" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="433" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A433" s="1" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B433" s="1" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C433" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D433" s="5" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E433" s="5" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F433" s="5">
+        <v>6</v>
+      </c>
+      <c r="G433" s="5" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="434" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A434" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B434" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C434" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D434" s="5" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E434" s="5" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F434" s="5">
+        <v>6</v>
+      </c>
+      <c r="G434" s="5" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="435" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A435" s="1" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B435" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C435" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D435" s="5" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E435" s="5" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F435" s="5">
+        <v>6</v>
+      </c>
+      <c r="G435" s="5" t="s">
+        <v>1217</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>